<commit_message>
add Vinst for Aeris instruments
</commit_message>
<xml_diff>
--- a/docs/example_auxfile.xlsx
+++ b/docs/example_auxfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\goFlux-workshop\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\goFlux-webpage\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CCF02C-ACA1-493A-84A3-CFCDF46166F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924DDB16-D332-4E65-B8B4-7089CC7C4372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{37EAA392-8239-4937-80C2-5CD3FC179F41}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>UniqueID</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>LGR N2OM1</t>
+  </si>
+  <si>
+    <t>Aeris MIRA Ultra CH4/C2H6</t>
+  </si>
+  <si>
+    <t>Aeris MIRA Ultra N2O/CO2</t>
+  </si>
+  <si>
+    <t>Gasmet GT5000</t>
   </si>
 </sst>
 </file>
@@ -196,7 +205,7 @@
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +223,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -254,6 +270,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -321,9 +338,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -361,7 +378,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -467,7 +484,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -609,7 +626,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,7 +706,7 @@
         <v>5.6999999999999993</v>
       </c>
       <c r="G2" s="13">
-        <f>'Vinst &amp; Vcham'!$C$13</f>
+        <f>'Vinst &amp; Vcham'!$C$14</f>
         <v>4244.1000000000004</v>
       </c>
       <c r="H2" s="12">
@@ -732,7 +749,7 @@
         <v>4.7</v>
       </c>
       <c r="G3" s="13">
-        <f>'Vinst &amp; Vcham'!$C$13</f>
+        <f>'Vinst &amp; Vcham'!$C$14</f>
         <v>4244.1000000000004</v>
       </c>
       <c r="H3" s="12">
@@ -775,7 +792,7 @@
         <v>6.4250000000000007</v>
       </c>
       <c r="G4" s="13">
-        <f>'Vinst &amp; Vcham'!$C$13</f>
+        <f>'Vinst &amp; Vcham'!$C$14</f>
         <v>4244.1000000000004</v>
       </c>
       <c r="H4" s="12">
@@ -818,7 +835,7 @@
         <v>3.9749999999999996</v>
       </c>
       <c r="G5" s="13">
-        <f>'Vinst &amp; Vcham'!$C$13</f>
+        <f>'Vinst &amp; Vcham'!$C$14</f>
         <v>4244.1000000000004</v>
       </c>
       <c r="H5" s="12">
@@ -861,7 +878,7 @@
         <v>5.1750000000000007</v>
       </c>
       <c r="G6" s="13">
-        <f>'Vinst &amp; Vcham'!$C$13</f>
+        <f>'Vinst &amp; Vcham'!$C$14</f>
         <v>4244.1000000000004</v>
       </c>
       <c r="H6" s="12">
@@ -904,7 +921,7 @@
         <v>6.3000000000000007</v>
       </c>
       <c r="G7" s="13">
-        <f>'Vinst &amp; Vcham'!$C$13</f>
+        <f>'Vinst &amp; Vcham'!$C$14</f>
         <v>4244.1000000000004</v>
       </c>
       <c r="H7" s="12">
@@ -1063,13 +1080,15 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
@@ -1123,23 +1142,23 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>13</v>
+        <v>51</v>
+      </c>
+      <c r="B6" s="14">
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>35</v>
@@ -1147,23 +1166,23 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
-        <v>90</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
-        <v>6.4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>6.4</v>
@@ -1171,30 +1190,54 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13">
-        <v>4244.1000000000004</v>
-      </c>
-      <c r="D13">
-        <v>324</v>
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>4244.1000000000004</v>
+      </c>
+      <c r="D14">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B14">
-        <f>45+B10+B11</f>
+      <c r="B15">
+        <f>45+B11+B12</f>
         <v>57.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new instrument volume provided
</commit_message>
<xml_diff>
--- a/docs/example_auxfile.xlsx
+++ b/docs/example_auxfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\goFlux-webpage\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsn874\Documents\goFlux-webpage\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F047FF-0497-4D9C-AD2D-87E0713DCE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF590334-38E9-421E-B179-6785EE79C120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="2520" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{37EAA392-8239-4937-80C2-5CD3FC179F41}"/>
+    <workbookView xWindow="1824" yWindow="3144" windowWidth="23040" windowHeight="9528" activeTab="2" xr2:uid="{37EAA392-8239-4937-80C2-5CD3FC179F41}"/>
   </bookViews>
   <sheets>
     <sheet name="auxfile" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>UniqueID</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>You can add any other columns relevant to your study to this file. They will be included in the outputs from the obs.win() and click.peak2() functions.</t>
+  </si>
+  <si>
+    <t>Eosense eosMX12</t>
   </si>
 </sst>
 </file>
@@ -708,16 +711,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" style="7" customWidth="1"/>
-    <col min="5" max="12" width="9.81640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="7" customWidth="1"/>
+    <col min="5" max="12" width="9.77734375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -755,7 +758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -798,7 +801,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -841,7 +844,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -884,7 +887,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -927,7 +930,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -970,7 +973,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1031,13 +1034,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" customWidth="1"/>
-    <col min="2" max="2" width="123.6328125" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="123.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
@@ -1125,7 +1128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
@@ -1152,21 +1155,21 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1183,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1236,12 +1239,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>57.8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1352,12 +1355,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
       <c r="B23">
         <v>640</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>